<commit_message>
Updated version of Bosses Improved display for bosses Fixed some powers Fixed some pokemon displays Adding new pokemons
</commit_message>
<xml_diff>
--- a/src/resources/AllCompetences.xlsx
+++ b/src/resources/AllCompetences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/pokemon-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEE5294-9B48-7D46-89FF-382EB6DADBCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432574FA-FFB9-314A-8F6F-DE4ECD80CD32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="966">
   <si>
     <t>Competence</t>
   </si>
@@ -3028,6 +3028,9 @@
   </si>
   <si>
     <t>Attaque prioritaire. Plein de dents attaquent le pokemon et l'apeurent avec une precision de 4 empechant l'adversaire d'attaquer ce tour.</t>
+  </si>
+  <si>
+    <t>Laser Glace gele l'ennemi avec une precision de 1. Le pokemon ne peut plus attaquer sauf avec une capacite de type feu qui le degele.</t>
   </si>
 </sst>
 </file>
@@ -4942,8 +4945,9 @@
   <autoFilter ref="A1:G690" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Lechouille"/>
-        <filter val="Mâchouille"/>
+        <filter val="Laser Glace"/>
+        <filter val="Laser Infinimax"/>
+        <filter val="Ultralaser"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4966,8 +4970,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:F234" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:F234" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:F235" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:F235" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Competence" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CType" dataCellStyle="Normal">
@@ -5311,7 +5315,7 @@
   <dimension ref="A1:G690"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+      <selection activeCell="G458" sqref="G458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7573,7 +7577,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" t="s">
         <v>529</v>
       </c>
@@ -8701,7 +8705,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" t="s">
         <v>560</v>
       </c>
@@ -15491,7 +15495,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="457" spans="1:7" hidden="1">
+    <row r="457" spans="1:7">
       <c r="A457" t="s">
         <v>272</v>
       </c>
@@ -15507,12 +15511,15 @@
       <c r="E457">
         <v>100</v>
       </c>
-      <c r="F457" t="e">
-        <f>VLOOKUP(Table1[[#This Row],[Competence]],'A copier'!A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="458" spans="1:7" hidden="1">
+      <c r="F457" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[Competence]],'A copier'!A:A,1,FALSE)</f>
+        <v>Laser Glace</v>
+      </c>
+      <c r="G457" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7">
       <c r="A458" t="s">
         <v>233</v>
       </c>
@@ -19679,7 +19686,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="653" spans="1:6" hidden="1">
+    <row r="653" spans="1:6">
       <c r="A653" t="s">
         <v>505</v>
       </c>
@@ -20521,10 +20528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G234"/>
+  <dimension ref="A1:G235"/>
   <sheetViews>
-    <sheetView topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A234" sqref="A234"/>
+    <sheetView topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="F235" sqref="F235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26361,6 +26368,31 @@
       <c r="F234" s="2" t="str">
         <f>VLOOKUP(Table3[[#This Row],[Competence]],Table1[],7,FALSE)</f>
         <v>Attaque prioritaire. Plein de dents attaquent le pokemon et l'apeurent avec une precision de 4 empechant l'adversaire d'attaquer ce tour.</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B235" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Competence]],Table1[],2,FALSE)</f>
+        <v>Glace</v>
+      </c>
+      <c r="C235" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Competence]],Table1[],3,FALSE)</f>
+        <v>Special</v>
+      </c>
+      <c r="D235" s="2">
+        <f>ROUND(VLOOKUP(Table3[[#This Row],[Competence]],Table1[],4,FALSE)/10,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E235" s="2">
+        <f>MAX(ROUND(((VLOOKUP(Table3[[#This Row],[Competence]],Table1[],5,FALSE)-55)/5+1)/10*6,0),0)</f>
+        <v>6</v>
+      </c>
+      <c r="F235" s="2" t="str">
+        <f>VLOOKUP(Table3[[#This Row],[Competence]],Table1[],7,FALSE)</f>
+        <v>Laser Glace gele l'ennemi avec une precision de 1. Le pokemon ne peut plus attaquer sauf avec une capacite de type feu qui le degele.</v>
       </c>
     </row>
   </sheetData>
@@ -26384,7 +26416,7 @@
   <dimension ref="A1:J213"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>